<commit_message>
Fix missing unit in variable template
</commit_message>
<xml_diff>
--- a/attachments/2021-07-09_template_Ariadne.xlsx
+++ b/attachments/2021-07-09_template_Ariadne.xlsx
@@ -16,7 +16,7 @@
     <sheet name="comments " sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">variable_definitions!$A$1:$E$1255</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">variable_definitions!$A$1:$E$1850</definedName>
     <definedName function="false" hidden="false" name="AreaUnderMACYN" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="BioenergyCropsYN" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="BurdenSharing" vbProcedure="false">#REF!</definedName>
@@ -107,6 +107,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="WhenFlex" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="WhenFlex2" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="YN" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">variable_definitions!$A$1:$E$1255</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">data!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7605" uniqueCount="3898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7606" uniqueCount="3898">
   <si>
     <t xml:space="preserve">General Instructions</t>
   </si>
@@ -12359,12 +12360,12 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="1" sqref="D941 B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="111"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="2" width="9.18"/>
@@ -12637,14 +12638,14 @@
   <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D941 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="79.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="79.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13315,9 +13316,9 @@
   <dimension ref="A1:E1850"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A1548" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A935" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1563" activeCellId="0" sqref="C1563"/>
+      <selection pane="bottomLeft" activeCell="D941" activeCellId="0" sqref="D941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29320,7 +29321,9 @@
       <c r="C941" s="26" t="s">
         <v>2097</v>
       </c>
-      <c r="D941" s="26"/>
+      <c r="D941" s="26" t="s">
+        <v>1195</v>
+      </c>
       <c r="E941" s="27" t="s">
         <v>2098</v>
       </c>
@@ -44779,7 +44782,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1255"/>
+  <autoFilter ref="A1:E1850"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -44800,13 +44803,13 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D941 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.91"/>
   </cols>
@@ -44848,7 +44851,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="D941 D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45184,14 +45187,14 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+      <selection pane="topLeft" activeCell="F37" activeCellId="1" sqref="D941 F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="34.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="87.45"/>

</xml_diff>

<commit_message>
Fix missing unit in variable template (#25)
</commit_message>
<xml_diff>
--- a/attachments/2021-07-09_template_Ariadne.xlsx
+++ b/attachments/2021-07-09_template_Ariadne.xlsx
@@ -16,7 +16,7 @@
     <sheet name="comments " sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">variable_definitions!$A$1:$E$1255</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">variable_definitions!$A$1:$E$1850</definedName>
     <definedName function="false" hidden="false" name="AreaUnderMACYN" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="BioenergyCropsYN" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="BurdenSharing" vbProcedure="false">#REF!</definedName>
@@ -107,6 +107,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="WhenFlex" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="WhenFlex2" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="YN" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">variable_definitions!$A$1:$E$1255</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">data!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7605" uniqueCount="3898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7606" uniqueCount="3898">
   <si>
     <t xml:space="preserve">General Instructions</t>
   </si>
@@ -12359,12 +12360,12 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="1" sqref="D941 B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="111"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="2" width="9.18"/>
@@ -12637,14 +12638,14 @@
   <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D941 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="79.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="79.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13315,9 +13316,9 @@
   <dimension ref="A1:E1850"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A1548" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A935" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1563" activeCellId="0" sqref="C1563"/>
+      <selection pane="bottomLeft" activeCell="D941" activeCellId="0" sqref="D941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29320,7 +29321,9 @@
       <c r="C941" s="26" t="s">
         <v>2097</v>
       </c>
-      <c r="D941" s="26"/>
+      <c r="D941" s="26" t="s">
+        <v>1195</v>
+      </c>
       <c r="E941" s="27" t="s">
         <v>2098</v>
       </c>
@@ -44779,7 +44782,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1255"/>
+  <autoFilter ref="A1:E1850"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -44800,13 +44803,13 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D941 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.91"/>
   </cols>
@@ -44848,7 +44851,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="1" sqref="D941 D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45184,14 +45187,14 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+      <selection pane="topLeft" activeCell="F37" activeCellId="1" sqref="D941 F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="34.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="87.45"/>

</xml_diff>